<commit_message>
minor corrections of print and presentation
</commit_message>
<xml_diff>
--- a/Mappe1.xlsx
+++ b/Mappe1.xlsx
@@ -3,16 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Vinz\GOs\GopherPEDS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26580" windowHeight="14016"/>
+    <workbookView windowHeight="14016" windowWidth="26580" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="TermExtList" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>publnos</t>
   </si>
@@ -45,16 +41,86 @@
   </si>
   <si>
     <t>US10272200 BB</t>
+  </si>
+  <si>
+    <t>Publ. No</t>
+  </si>
+  <si>
+    <t>Term Ext. [days]</t>
+  </si>
+  <si>
+    <t>Disclaimer/Date</t>
+  </si>
+  <si>
+    <t>Appl ID</t>
+  </si>
+  <si>
+    <t>US20190107969A1</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>Terminal Disclaimer Filed2020-09-14 00:00:00</t>
+  </si>
+  <si>
+    <t>16204798</t>
+  </si>
+  <si>
+    <t>10272200</t>
+  </si>
+  <si>
+    <t>no extension</t>
+  </si>
+  <si>
+    <t>no disclaimer</t>
+  </si>
+  <si>
+    <t>15114834</t>
+  </si>
+  <si>
+    <t>US20210236729A1</t>
+  </si>
+  <si>
+    <t>17161528</t>
+  </si>
+  <si>
+    <t>US20210038163A1</t>
+  </si>
+  <si>
+    <t>16533470</t>
+  </si>
+  <si>
+    <t>9974492</t>
+  </si>
+  <si>
+    <t>15255909</t>
+  </si>
+  <si>
+    <t>10185513</t>
+  </si>
+  <si>
+    <t>167</t>
+  </si>
+  <si>
+    <t>15256137</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -79,14 +145,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="false">
+      <alignment/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -408,4 +477,116 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col customWidth="true" max="4" min="1" width="30"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>